<commit_message>
Asignación de autores recursos en greco Mat 7 tema 10
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion10/Escaleta_MA_07_10_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion10/Escaleta_MA_07_10_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion10\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="292">
   <si>
     <t>Asignatura</t>
   </si>
@@ -892,6 +892,12 @@
   </si>
   <si>
     <t>Recurso M102AB-01</t>
+  </si>
+  <si>
+    <t>Johanna Vera</t>
+  </si>
+  <si>
+    <t>Adriana Lasprilla</t>
   </si>
 </sst>
 </file>
@@ -1278,8 +1284,32 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1320,30 +1350,6 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5936,8 +5942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR1093"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="W26" sqref="W26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5970,96 +5976,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" s="32" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="63" t="s">
+      <c r="D1" s="73" t="s">
         <v>214</v>
       </c>
-      <c r="E1" s="65" t="s">
+      <c r="E1" s="75" t="s">
         <v>215</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="77" t="s">
         <v>216</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="67" t="s">
+      <c r="H1" s="77" t="s">
         <v>217</v>
       </c>
-      <c r="I1" s="67" t="s">
+      <c r="I1" s="77" t="s">
         <v>202</v>
       </c>
-      <c r="J1" s="60" t="s">
+      <c r="J1" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="59" t="s">
+      <c r="K1" s="69" t="s">
         <v>212</v>
       </c>
-      <c r="L1" s="58" t="s">
+      <c r="L1" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="61" t="s">
+      <c r="M1" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="61"/>
-      <c r="O1" s="55" t="s">
+      <c r="N1" s="71"/>
+      <c r="O1" s="61" t="s">
         <v>266</v>
       </c>
-      <c r="P1" s="55" t="s">
+      <c r="P1" s="61" t="s">
         <v>213</v>
       </c>
-      <c r="Q1" s="72" t="s">
+      <c r="Q1" s="65" t="s">
         <v>119</v>
       </c>
-      <c r="R1" s="71" t="s">
+      <c r="R1" s="64" t="s">
         <v>120</v>
       </c>
-      <c r="S1" s="69" t="s">
+      <c r="S1" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="T1" s="70" t="s">
+      <c r="T1" s="63" t="s">
         <v>122</v>
       </c>
-      <c r="U1" s="69" t="s">
+      <c r="U1" s="62" t="s">
         <v>123</v>
       </c>
       <c r="W1" s="49"/>
       <c r="X1" s="49"/>
     </row>
     <row r="2" spans="1:44" s="32" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="58"/>
+      <c r="A2" s="67"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="68"/>
       <c r="M2" s="33" t="s">
         <v>124</v>
       </c>
       <c r="N2" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="72"/>
-      <c r="R2" s="71"/>
-      <c r="S2" s="69"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="69"/>
+      <c r="O2" s="61"/>
+      <c r="P2" s="61"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="64"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="62"/>
       <c r="W2" s="49"/>
       <c r="X2" s="49"/>
     </row>
@@ -6104,19 +6110,19 @@
       <c r="P3" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="Q3" s="74">
+      <c r="Q3" s="56">
         <v>7</v>
       </c>
-      <c r="R3" s="74" t="s">
+      <c r="R3" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="S3" s="74" t="s">
+      <c r="S3" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="T3" s="74" t="s">
+      <c r="T3" s="56" t="s">
         <v>218</v>
       </c>
-      <c r="U3" s="74" t="s">
+      <c r="U3" s="56" t="s">
         <v>268</v>
       </c>
       <c r="V3" s="49"/>
@@ -6162,19 +6168,19 @@
       <c r="P4" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="Q4" s="74">
+      <c r="Q4" s="56">
         <v>7</v>
       </c>
-      <c r="R4" s="74" t="s">
+      <c r="R4" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="S4" s="74" t="s">
+      <c r="S4" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="T4" s="74" t="s">
+      <c r="T4" s="56" t="s">
         <v>219</v>
       </c>
-      <c r="U4" s="74" t="s">
+      <c r="U4" s="56" t="s">
         <v>268</v>
       </c>
       <c r="V4" s="49"/>
@@ -6220,19 +6226,19 @@
       <c r="P5" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="Q5" s="74">
+      <c r="Q5" s="56">
         <v>7</v>
       </c>
-      <c r="R5" s="74" t="s">
+      <c r="R5" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="S5" s="74" t="s">
+      <c r="S5" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="T5" s="74" t="s">
+      <c r="T5" s="56" t="s">
         <v>269</v>
       </c>
-      <c r="U5" s="74" t="s">
+      <c r="U5" s="56" t="s">
         <v>268</v>
       </c>
       <c r="V5" s="49"/>
@@ -6277,19 +6283,19 @@
       <c r="P6" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="Q6" s="74">
+      <c r="Q6" s="56">
         <v>7</v>
       </c>
-      <c r="R6" s="74" t="s">
+      <c r="R6" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="S6" s="74" t="s">
+      <c r="S6" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="T6" s="74" t="s">
+      <c r="T6" s="56" t="s">
         <v>251</v>
       </c>
-      <c r="U6" s="74" t="s">
+      <c r="U6" s="56" t="s">
         <v>268</v>
       </c>
       <c r="V6" s="35"/>
@@ -6302,7 +6308,7 @@
       <c r="D7" s="41"/>
       <c r="E7" s="40"/>
       <c r="F7" s="39"/>
-      <c r="G7" s="73" t="s">
+      <c r="G7" s="55" t="s">
         <v>277</v>
       </c>
       <c r="H7" s="43"/>
@@ -6328,19 +6334,19 @@
       <c r="P7" s="44" t="s">
         <v>204</v>
       </c>
-      <c r="Q7" s="74">
+      <c r="Q7" s="56">
         <v>6</v>
       </c>
-      <c r="R7" s="74" t="s">
+      <c r="R7" s="56" t="s">
         <v>280</v>
       </c>
-      <c r="S7" s="74" t="s">
+      <c r="S7" s="56" t="s">
         <v>281</v>
       </c>
-      <c r="T7" s="75" t="s">
+      <c r="T7" s="57" t="s">
         <v>282</v>
       </c>
-      <c r="U7" s="74" t="s">
+      <c r="U7" s="56" t="s">
         <v>283</v>
       </c>
       <c r="V7" s="35"/>
@@ -6385,19 +6391,19 @@
       <c r="P8" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="Q8" s="74">
+      <c r="Q8" s="56">
         <v>7</v>
       </c>
-      <c r="R8" s="74" t="s">
+      <c r="R8" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="S8" s="74" t="s">
+      <c r="S8" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="T8" s="74" t="s">
+      <c r="T8" s="56" t="s">
         <v>221</v>
       </c>
-      <c r="U8" s="74" t="s">
+      <c r="U8" s="56" t="s">
         <v>268</v>
       </c>
       <c r="V8" s="49"/>
@@ -6441,19 +6447,19 @@
       <c r="P9" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="Q9" s="74">
+      <c r="Q9" s="56">
         <v>7</v>
       </c>
-      <c r="R9" s="74" t="s">
+      <c r="R9" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="S9" s="74" t="s">
+      <c r="S9" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="T9" s="74" t="s">
+      <c r="T9" s="56" t="s">
         <v>270</v>
       </c>
-      <c r="U9" s="74" t="s">
+      <c r="U9" s="56" t="s">
         <v>268</v>
       </c>
       <c r="V9" s="49"/>
@@ -6519,19 +6525,19 @@
       <c r="P10" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="Q10" s="74">
+      <c r="Q10" s="56">
         <v>7</v>
       </c>
-      <c r="R10" s="74" t="s">
+      <c r="R10" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="S10" s="74" t="s">
+      <c r="S10" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="T10" s="74" t="s">
+      <c r="T10" s="56" t="s">
         <v>233</v>
       </c>
-      <c r="U10" s="74" t="s">
+      <c r="U10" s="56" t="s">
         <v>268</v>
       </c>
       <c r="V10" s="49"/>
@@ -6577,19 +6583,19 @@
       <c r="P11" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="Q11" s="74">
+      <c r="Q11" s="56">
         <v>7</v>
       </c>
-      <c r="R11" s="74" t="s">
+      <c r="R11" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="S11" s="74" t="s">
+      <c r="S11" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="T11" s="74" t="s">
+      <c r="T11" s="56" t="s">
         <v>252</v>
       </c>
-      <c r="U11" s="74" t="s">
+      <c r="U11" s="56" t="s">
         <v>268</v>
       </c>
       <c r="V11" s="35"/>
@@ -6634,19 +6640,19 @@
       <c r="P12" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="Q12" s="74">
+      <c r="Q12" s="56">
         <v>7</v>
       </c>
-      <c r="R12" s="74" t="s">
+      <c r="R12" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="S12" s="74" t="s">
+      <c r="S12" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="T12" s="74" t="s">
+      <c r="T12" s="56" t="s">
         <v>223</v>
       </c>
-      <c r="U12" s="74" t="s">
+      <c r="U12" s="56" t="s">
         <v>268</v>
       </c>
       <c r="V12" s="49"/>
@@ -6690,19 +6696,19 @@
       <c r="P13" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="Q13" s="74">
+      <c r="Q13" s="56">
         <v>7</v>
       </c>
-      <c r="R13" s="74" t="s">
+      <c r="R13" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="S13" s="74" t="s">
+      <c r="S13" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="T13" s="74" t="s">
+      <c r="T13" s="56" t="s">
         <v>224</v>
       </c>
-      <c r="U13" s="74" t="s">
+      <c r="U13" s="56" t="s">
         <v>274</v>
       </c>
       <c r="V13" s="49"/>
@@ -6768,19 +6774,19 @@
       <c r="P14" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="Q14" s="74">
+      <c r="Q14" s="56">
         <v>7</v>
       </c>
-      <c r="R14" s="74" t="s">
+      <c r="R14" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="S14" s="74" t="s">
+      <c r="S14" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="T14" s="74" t="s">
+      <c r="T14" s="56" t="s">
         <v>225</v>
       </c>
-      <c r="U14" s="74" t="s">
+      <c r="U14" s="56" t="s">
         <v>268</v>
       </c>
       <c r="V14" s="49"/>
@@ -6825,19 +6831,19 @@
       <c r="P15" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="Q15" s="74">
+      <c r="Q15" s="56">
         <v>7</v>
       </c>
-      <c r="R15" s="74" t="s">
+      <c r="R15" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="S15" s="74" t="s">
+      <c r="S15" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="T15" s="74" t="s">
+      <c r="T15" s="56" t="s">
         <v>228</v>
       </c>
-      <c r="U15" s="74" t="s">
+      <c r="U15" s="56" t="s">
         <v>268</v>
       </c>
       <c r="V15" s="35"/>
@@ -6881,19 +6887,19 @@
       <c r="P16" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="Q16" s="74">
+      <c r="Q16" s="56">
         <v>7</v>
       </c>
-      <c r="R16" s="74" t="s">
+      <c r="R16" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="S16" s="74" t="s">
+      <c r="S16" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="T16" s="74" t="s">
+      <c r="T16" s="56" t="s">
         <v>275</v>
       </c>
-      <c r="U16" s="74" t="s">
+      <c r="U16" s="56" t="s">
         <v>274</v>
       </c>
       <c r="V16" s="35"/>
@@ -6937,19 +6943,19 @@
       <c r="P17" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="Q17" s="74">
+      <c r="Q17" s="56">
         <v>7</v>
       </c>
-      <c r="R17" s="74" t="s">
+      <c r="R17" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="S17" s="74" t="s">
+      <c r="S17" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="T17" s="74" t="s">
+      <c r="T17" s="56" t="s">
         <v>253</v>
       </c>
-      <c r="U17" s="74" t="s">
+      <c r="U17" s="56" t="s">
         <v>268</v>
       </c>
       <c r="X17" s="52"/>
@@ -6993,19 +6999,19 @@
       <c r="P18" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="Q18" s="74">
+      <c r="Q18" s="56">
         <v>7</v>
       </c>
-      <c r="R18" s="74" t="s">
+      <c r="R18" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="S18" s="74" t="s">
+      <c r="S18" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="T18" s="74" t="s">
+      <c r="T18" s="56" t="s">
         <v>276</v>
       </c>
-      <c r="U18" s="74" t="s">
+      <c r="U18" s="56" t="s">
         <v>274</v>
       </c>
       <c r="V18"/>
@@ -7050,19 +7056,19 @@
       <c r="P19" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="Q19" s="74">
+      <c r="Q19" s="56">
         <v>7</v>
       </c>
-      <c r="R19" s="74" t="s">
+      <c r="R19" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="S19" s="74" t="s">
+      <c r="S19" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="T19" s="74" t="s">
+      <c r="T19" s="56" t="s">
         <v>254</v>
       </c>
-      <c r="U19" s="74" t="s">
+      <c r="U19" s="56" t="s">
         <v>268</v>
       </c>
       <c r="V19" s="35"/>
@@ -7107,19 +7113,19 @@
       <c r="P20" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="Q20" s="74">
+      <c r="Q20" s="56">
         <v>7</v>
       </c>
-      <c r="R20" s="74" t="s">
+      <c r="R20" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="S20" s="74" t="s">
+      <c r="S20" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="T20" s="74" t="s">
+      <c r="T20" s="56" t="s">
         <v>271</v>
       </c>
-      <c r="U20" s="74" t="s">
+      <c r="U20" s="56" t="s">
         <v>268</v>
       </c>
       <c r="V20" s="49"/>
@@ -7164,19 +7170,19 @@
       <c r="P21" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="Q21" s="74">
+      <c r="Q21" s="56">
         <v>7</v>
       </c>
-      <c r="R21" s="74" t="s">
+      <c r="R21" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="S21" s="74" t="s">
+      <c r="S21" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="T21" s="74" t="s">
+      <c r="T21" s="56" t="s">
         <v>273</v>
       </c>
-      <c r="U21" s="74" t="s">
+      <c r="U21" s="56" t="s">
         <v>268</v>
       </c>
       <c r="V21" s="49"/>
@@ -7225,22 +7231,24 @@
       <c r="P22" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="Q22" s="74">
+      <c r="Q22" s="56">
         <v>6</v>
       </c>
-      <c r="R22" s="74" t="s">
+      <c r="R22" s="56" t="s">
         <v>284</v>
       </c>
-      <c r="S22" s="74" t="s">
+      <c r="S22" s="56" t="s">
         <v>285</v>
       </c>
-      <c r="T22" s="75" t="s">
+      <c r="T22" s="57" t="s">
         <v>289</v>
       </c>
-      <c r="U22" s="74" t="s">
+      <c r="U22" s="56" t="s">
         <v>287</v>
       </c>
-      <c r="V22" s="35"/>
+      <c r="V22" s="35" t="s">
+        <v>290</v>
+      </c>
       <c r="W22" s="51"/>
     </row>
     <row r="23" spans="1:38" x14ac:dyDescent="0.25">
@@ -7280,14 +7288,14 @@
       <c r="P23" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="Q23" s="76"/>
-      <c r="R23" s="77"/>
-      <c r="S23" s="77"/>
-      <c r="T23" s="77"/>
-      <c r="U23" s="77"/>
+      <c r="Q23" s="58"/>
+      <c r="R23" s="59"/>
+      <c r="S23" s="59"/>
+      <c r="T23" s="59"/>
+      <c r="U23" s="59"/>
       <c r="V23" s="35"/>
     </row>
-    <row r="24" spans="1:38" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" s="37" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="39" t="s">
         <v>76</v>
       </c>
@@ -7328,22 +7336,24 @@
       <c r="P24" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="Q24" s="74">
+      <c r="Q24" s="56">
         <v>6</v>
       </c>
-      <c r="R24" s="74" t="s">
+      <c r="R24" s="56" t="s">
         <v>284</v>
       </c>
-      <c r="S24" s="74" t="s">
+      <c r="S24" s="56" t="s">
         <v>285</v>
       </c>
-      <c r="T24" s="75" t="s">
+      <c r="T24" s="57" t="s">
         <v>286</v>
       </c>
-      <c r="U24" s="74" t="s">
+      <c r="U24" s="56" t="s">
         <v>287</v>
       </c>
-      <c r="V24" s="49"/>
+      <c r="V24" s="49" t="s">
+        <v>291</v>
+      </c>
       <c r="W24" s="35"/>
       <c r="X24" s="35"/>
       <c r="Y24" s="35"/>
@@ -7400,19 +7410,19 @@
       <c r="P25" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="Q25" s="74">
+      <c r="Q25" s="56">
         <v>7</v>
       </c>
-      <c r="R25" s="74" t="s">
+      <c r="R25" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="S25" s="74" t="s">
+      <c r="S25" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="T25" s="74" t="s">
+      <c r="T25" s="56" t="s">
         <v>272</v>
       </c>
-      <c r="U25" s="74" t="s">
+      <c r="U25" s="56" t="s">
         <v>274</v>
       </c>
       <c r="V25"/>
@@ -7461,11 +7471,11 @@
       <c r="N27" s="39"/>
       <c r="O27" s="42"/>
       <c r="P27" s="44"/>
-      <c r="Q27" s="78"/>
-      <c r="R27" s="78"/>
-      <c r="S27" s="78"/>
-      <c r="T27" s="78"/>
-      <c r="U27" s="78"/>
+      <c r="Q27" s="60"/>
+      <c r="R27" s="60"/>
+      <c r="S27" s="60"/>
+      <c r="T27" s="60"/>
+      <c r="U27" s="60"/>
       <c r="V27" s="49"/>
       <c r="W27" s="51"/>
       <c r="X27" s="52"/>
@@ -11690,12 +11700,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
@@ -11710,6 +11714,12 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K40">

</xml_diff>

<commit_message>
Actualización guion 10 finalizado
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion10/Escaleta_MA_07_10_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion10/Escaleta_MA_07_10_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johana Montejo Rozo\Desktop\Edicion\guion10\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="7215"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -469,9 +474,6 @@
     <t>Actividades sobre el concepto de función</t>
   </si>
   <si>
-    <t>Actividades sobre La representación gráfica de funciones</t>
-  </si>
-  <si>
     <t>Actividades sobre La modelación de problemas mediante funciones</t>
   </si>
   <si>
@@ -545,6 +547,9 @@
   </si>
   <si>
     <t>¿Que sabes de la funciones?</t>
+  </si>
+  <si>
+    <t>Actividad que sirve para int+J19erprestar la representación gráfica de una función</t>
   </si>
 </sst>
 </file>
@@ -805,7 +810,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -888,9 +893,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -921,10 +923,48 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -933,53 +973,21 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1040,7 +1048,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1075,7 +1083,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1286,8 +1294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR1093"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" topLeftCell="H13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1320,98 +1328,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" s="32" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="71" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="73" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="60" t="s">
+      <c r="F1" s="75" t="s">
         <v>102</v>
       </c>
-      <c r="G1" s="61" t="s">
+      <c r="G1" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="60" t="s">
+      <c r="H1" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="I1" s="60" t="s">
+      <c r="I1" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="J1" s="62" t="s">
+      <c r="J1" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="63" t="s">
+      <c r="K1" s="67" t="s">
         <v>98</v>
       </c>
-      <c r="L1" s="61" t="s">
+      <c r="L1" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="64" t="s">
+      <c r="M1" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="64"/>
-      <c r="O1" s="65" t="s">
-        <v>152</v>
-      </c>
-      <c r="P1" s="65" t="s">
+      <c r="N1" s="69"/>
+      <c r="O1" s="59" t="s">
+        <v>151</v>
+      </c>
+      <c r="P1" s="59" t="s">
         <v>99</v>
       </c>
-      <c r="Q1" s="66" t="s">
+      <c r="Q1" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="R1" s="67" t="s">
+      <c r="R1" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="S1" s="68" t="s">
+      <c r="S1" s="60" t="s">
         <v>82</v>
       </c>
-      <c r="T1" s="69" t="s">
+      <c r="T1" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="U1" s="68" t="s">
+      <c r="U1" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
     </row>
     <row r="2" spans="1:44" s="32" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="73" t="s">
+      <c r="A2" s="65"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="N2" s="73" t="s">
+      <c r="N2" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="67"/>
-      <c r="S2" s="68"/>
-      <c r="T2" s="69"/>
-      <c r="U2" s="68"/>
-      <c r="W2" s="45"/>
-      <c r="X2" s="45"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="61"/>
+      <c r="U2" s="60"/>
+      <c r="W2" s="44"/>
+      <c r="X2" s="44"/>
     </row>
     <row r="3" spans="1:44" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -1426,15 +1434,15 @@
       <c r="D3" s="38" t="s">
         <v>144</v>
       </c>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="43" t="s">
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="H3" s="44">
+      <c r="H3" s="43">
         <v>1</v>
       </c>
-      <c r="I3" s="44" t="s">
+      <c r="I3" s="43" t="s">
         <v>89</v>
       </c>
       <c r="J3" s="38" t="s">
@@ -1449,29 +1457,29 @@
       <c r="M3" s="40"/>
       <c r="N3" s="40"/>
       <c r="O3" s="38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P3" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Q3" s="74">
+      <c r="Q3" s="55">
         <v>7</v>
       </c>
-      <c r="R3" s="74" t="s">
+      <c r="R3" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="S3" s="74" t="s">
+      <c r="S3" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="T3" s="55" t="s">
+        <v>104</v>
+      </c>
+      <c r="U3" s="55" t="s">
         <v>153</v>
       </c>
-      <c r="T3" s="74" t="s">
-        <v>104</v>
-      </c>
-      <c r="U3" s="74" t="s">
-        <v>154</v>
-      </c>
-      <c r="V3" s="45"/>
-      <c r="W3" s="45"/>
-      <c r="X3" s="46"/>
+      <c r="V3" s="44"/>
+      <c r="W3" s="44"/>
+      <c r="X3" s="45"/>
     </row>
     <row r="4" spans="1:44" s="32" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
@@ -1486,15 +1494,15 @@
       <c r="D4" s="38" t="s">
         <v>144</v>
       </c>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="43" t="s">
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="H4" s="44">
+      <c r="H4" s="43">
         <v>2</v>
       </c>
-      <c r="I4" s="44" t="s">
+      <c r="I4" s="43" t="s">
         <v>90</v>
       </c>
       <c r="J4" s="38" t="s">
@@ -1512,24 +1520,24 @@
       <c r="P4" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Q4" s="74">
+      <c r="Q4" s="55">
         <v>7</v>
       </c>
-      <c r="R4" s="74" t="s">
+      <c r="R4" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="S4" s="74" t="s">
+      <c r="S4" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="T4" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="U4" s="55" t="s">
         <v>153</v>
       </c>
-      <c r="T4" s="74" t="s">
-        <v>105</v>
-      </c>
-      <c r="U4" s="74" t="s">
-        <v>154</v>
-      </c>
-      <c r="V4" s="45"/>
-      <c r="W4" s="45"/>
-      <c r="X4" s="46"/>
+      <c r="V4" s="44"/>
+      <c r="W4" s="44"/>
+      <c r="X4" s="45"/>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="40" t="s">
@@ -1546,7 +1554,7 @@
       </c>
       <c r="E5" s="38"/>
       <c r="F5" s="40"/>
-      <c r="G5" s="38" t="s">
+      <c r="G5" s="58" t="s">
         <v>106</v>
       </c>
       <c r="H5" s="40">
@@ -1570,23 +1578,23 @@
       <c r="P5" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Q5" s="74">
+      <c r="Q5" s="55">
         <v>7</v>
       </c>
-      <c r="R5" s="74" t="s">
+      <c r="R5" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="S5" s="74" t="s">
+      <c r="S5" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="T5" s="55" t="s">
+        <v>154</v>
+      </c>
+      <c r="U5" s="55" t="s">
         <v>153</v>
       </c>
-      <c r="T5" s="74" t="s">
-        <v>155</v>
-      </c>
-      <c r="U5" s="74" t="s">
-        <v>154</v>
-      </c>
-      <c r="V5" s="45"/>
-      <c r="X5" s="46"/>
+      <c r="V5" s="44"/>
+      <c r="X5" s="45"/>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
@@ -1605,10 +1613,10 @@
         <v>92</v>
       </c>
       <c r="F6" s="40"/>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="58" t="s">
         <v>137</v>
       </c>
-      <c r="H6" s="44">
+      <c r="H6" s="43">
         <v>4</v>
       </c>
       <c r="I6" s="40" t="s">
@@ -1629,23 +1637,23 @@
       <c r="P6" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Q6" s="74">
+      <c r="Q6" s="55">
         <v>7</v>
       </c>
-      <c r="R6" s="74" t="s">
+      <c r="R6" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="S6" s="74" t="s">
+      <c r="S6" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="T6" s="55" t="s">
+        <v>137</v>
+      </c>
+      <c r="U6" s="55" t="s">
         <v>153</v>
       </c>
-      <c r="T6" s="74" t="s">
-        <v>137</v>
-      </c>
-      <c r="U6" s="74" t="s">
-        <v>154</v>
-      </c>
       <c r="V6" s="34"/>
-      <c r="X6" s="46"/>
+      <c r="X6" s="45"/>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="40" t="s">
@@ -1658,15 +1666,15 @@
       <c r="D7" s="38"/>
       <c r="E7" s="38"/>
       <c r="F7" s="40"/>
-      <c r="G7" s="51" t="s">
-        <v>175</v>
-      </c>
-      <c r="H7" s="44"/>
+      <c r="G7" s="50" t="s">
+        <v>174</v>
+      </c>
+      <c r="H7" s="43"/>
       <c r="I7" s="40" t="s">
         <v>89</v>
       </c>
       <c r="J7" s="39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K7" s="40" t="s">
         <v>90</v>
@@ -1679,28 +1687,28 @@
       </c>
       <c r="N7" s="40"/>
       <c r="O7" s="39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P7" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="Q7" s="74">
+      <c r="Q7" s="55">
         <v>6</v>
       </c>
-      <c r="R7" s="74" t="s">
+      <c r="R7" s="55" t="s">
+        <v>164</v>
+      </c>
+      <c r="S7" s="55" t="s">
         <v>165</v>
       </c>
-      <c r="S7" s="74" t="s">
+      <c r="T7" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="T7" s="52" t="s">
+      <c r="U7" s="55" t="s">
         <v>167</v>
       </c>
-      <c r="U7" s="74" t="s">
-        <v>168</v>
-      </c>
       <c r="V7" s="34"/>
-      <c r="X7" s="46"/>
+      <c r="X7" s="45"/>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
@@ -1717,10 +1725,10 @@
       </c>
       <c r="E8" s="38"/>
       <c r="F8" s="39"/>
-      <c r="G8" s="38" t="s">
+      <c r="G8" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="H8" s="44">
+      <c r="H8" s="43">
         <v>5</v>
       </c>
       <c r="I8" s="40" t="s">
@@ -1741,22 +1749,22 @@
       <c r="P8" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Q8" s="74">
+      <c r="Q8" s="55">
         <v>7</v>
       </c>
-      <c r="R8" s="74" t="s">
+      <c r="R8" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="S8" s="74" t="s">
+      <c r="S8" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="T8" s="55" t="s">
+        <v>107</v>
+      </c>
+      <c r="U8" s="55" t="s">
         <v>153</v>
       </c>
-      <c r="T8" s="74" t="s">
-        <v>107</v>
-      </c>
-      <c r="U8" s="74" t="s">
-        <v>154</v>
-      </c>
-      <c r="V8" s="45"/>
+      <c r="V8" s="44"/>
     </row>
     <row r="9" spans="1:44" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
@@ -1773,7 +1781,7 @@
       </c>
       <c r="E9" s="38"/>
       <c r="F9" s="39"/>
-      <c r="G9" s="38" t="s">
+      <c r="G9" s="58" t="s">
         <v>108</v>
       </c>
       <c r="H9" s="40">
@@ -1797,22 +1805,22 @@
       <c r="P9" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Q9" s="74">
+      <c r="Q9" s="55">
         <v>7</v>
       </c>
-      <c r="R9" s="74" t="s">
+      <c r="R9" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="S9" s="74" t="s">
+      <c r="S9" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="T9" s="55" t="s">
+        <v>155</v>
+      </c>
+      <c r="U9" s="55" t="s">
         <v>153</v>
       </c>
-      <c r="T9" s="74" t="s">
-        <v>156</v>
-      </c>
-      <c r="U9" s="74" t="s">
-        <v>154</v>
-      </c>
-      <c r="V9" s="45"/>
+      <c r="V9" s="44"/>
       <c r="W9" s="34"/>
       <c r="X9" s="34"/>
       <c r="Y9" s="34"/>
@@ -1851,10 +1859,10 @@
       </c>
       <c r="E10" s="38"/>
       <c r="F10" s="39"/>
-      <c r="G10" s="38" t="s">
+      <c r="G10" s="58" t="s">
         <v>119</v>
       </c>
-      <c r="H10" s="44">
+      <c r="H10" s="43">
         <v>7</v>
       </c>
       <c r="I10" s="40" t="s">
@@ -1875,24 +1883,24 @@
       <c r="P10" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Q10" s="74">
+      <c r="Q10" s="55">
         <v>7</v>
       </c>
-      <c r="R10" s="74" t="s">
+      <c r="R10" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="S10" s="74" t="s">
+      <c r="S10" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="T10" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="U10" s="55" t="s">
         <v>153</v>
       </c>
-      <c r="T10" s="74" t="s">
-        <v>119</v>
-      </c>
-      <c r="U10" s="74" t="s">
-        <v>154</v>
-      </c>
-      <c r="V10" s="45"/>
-      <c r="W10" s="47"/>
-      <c r="X10" s="48"/>
+      <c r="V10" s="44"/>
+      <c r="W10" s="46"/>
+      <c r="X10" s="47"/>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
@@ -1911,10 +1919,10 @@
         <v>92</v>
       </c>
       <c r="F11" s="39"/>
-      <c r="G11" s="38" t="s">
+      <c r="G11" s="58" t="s">
         <v>138</v>
       </c>
-      <c r="H11" s="44">
+      <c r="H11" s="43">
         <v>8</v>
       </c>
       <c r="I11" s="40" t="s">
@@ -1935,23 +1943,23 @@
       <c r="P11" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Q11" s="74">
+      <c r="Q11" s="55">
         <v>7</v>
       </c>
-      <c r="R11" s="74" t="s">
+      <c r="R11" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="S11" s="74" t="s">
+      <c r="S11" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="T11" s="55" t="s">
+        <v>138</v>
+      </c>
+      <c r="U11" s="55" t="s">
         <v>153</v>
       </c>
-      <c r="T11" s="74" t="s">
-        <v>138</v>
-      </c>
-      <c r="U11" s="74" t="s">
-        <v>154</v>
-      </c>
       <c r="V11" s="34"/>
-      <c r="X11" s="48"/>
+      <c r="X11" s="47"/>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
@@ -1968,7 +1976,7 @@
       </c>
       <c r="E12" s="39"/>
       <c r="F12" s="39"/>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="58" t="s">
         <v>109</v>
       </c>
       <c r="H12" s="40">
@@ -1992,22 +2000,22 @@
       <c r="P12" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Q12" s="74">
+      <c r="Q12" s="55">
         <v>7</v>
       </c>
-      <c r="R12" s="74" t="s">
+      <c r="R12" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="S12" s="74" t="s">
+      <c r="S12" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="T12" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="U12" s="55" t="s">
         <v>153</v>
       </c>
-      <c r="T12" s="74" t="s">
-        <v>109</v>
-      </c>
-      <c r="U12" s="74" t="s">
-        <v>154</v>
-      </c>
-      <c r="V12" s="45"/>
+      <c r="V12" s="44"/>
     </row>
     <row r="13" spans="1:44" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
@@ -2024,10 +2032,10 @@
       </c>
       <c r="E13" s="39"/>
       <c r="F13" s="39"/>
-      <c r="G13" s="38" t="s">
+      <c r="G13" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="H13" s="44">
+      <c r="H13" s="43">
         <v>10</v>
       </c>
       <c r="I13" s="40" t="s">
@@ -2048,22 +2056,22 @@
       <c r="P13" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Q13" s="74">
+      <c r="Q13" s="55">
         <v>7</v>
       </c>
-      <c r="R13" s="74" t="s">
+      <c r="R13" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="S13" s="74" t="s">
-        <v>153</v>
-      </c>
-      <c r="T13" s="74" t="s">
+      <c r="S13" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="T13" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="U13" s="74" t="s">
-        <v>160</v>
-      </c>
-      <c r="V13" s="45"/>
+      <c r="U13" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="V13" s="44"/>
       <c r="W13" s="34"/>
       <c r="X13" s="34"/>
       <c r="Y13" s="34"/>
@@ -2102,10 +2110,10 @@
       </c>
       <c r="E14" s="38"/>
       <c r="F14" s="39"/>
-      <c r="G14" s="38" t="s">
+      <c r="G14" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="H14" s="44">
+      <c r="H14" s="43">
         <v>11</v>
       </c>
       <c r="I14" s="40" t="s">
@@ -2126,23 +2134,23 @@
       <c r="P14" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Q14" s="74">
+      <c r="Q14" s="55">
         <v>7</v>
       </c>
-      <c r="R14" s="74" t="s">
+      <c r="R14" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="S14" s="74" t="s">
+      <c r="S14" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="T14" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="U14" s="55" t="s">
         <v>153</v>
       </c>
-      <c r="T14" s="74" t="s">
-        <v>111</v>
-      </c>
-      <c r="U14" s="74" t="s">
-        <v>154</v>
-      </c>
-      <c r="V14" s="45"/>
-      <c r="X14" s="49"/>
+      <c r="V14" s="44"/>
+      <c r="X14" s="48"/>
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
@@ -2159,7 +2167,7 @@
       </c>
       <c r="E15" s="39"/>
       <c r="F15" s="39"/>
-      <c r="G15" s="38" t="s">
+      <c r="G15" s="58" t="s">
         <v>114</v>
       </c>
       <c r="H15" s="40">
@@ -2183,20 +2191,20 @@
       <c r="P15" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Q15" s="74">
+      <c r="Q15" s="55">
         <v>7</v>
       </c>
-      <c r="R15" s="74" t="s">
+      <c r="R15" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="S15" s="74" t="s">
+      <c r="S15" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="T15" s="55" t="s">
+        <v>114</v>
+      </c>
+      <c r="U15" s="55" t="s">
         <v>153</v>
-      </c>
-      <c r="T15" s="74" t="s">
-        <v>114</v>
-      </c>
-      <c r="U15" s="74" t="s">
-        <v>154</v>
       </c>
       <c r="V15" s="34"/>
     </row>
@@ -2215,10 +2223,10 @@
       </c>
       <c r="E16" s="39"/>
       <c r="F16" s="39"/>
-      <c r="G16" s="38" t="s">
+      <c r="G16" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="H16" s="44">
+      <c r="H16" s="43">
         <v>13</v>
       </c>
       <c r="I16" s="40" t="s">
@@ -2239,20 +2247,20 @@
       <c r="P16" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Q16" s="74">
+      <c r="Q16" s="55">
         <v>7</v>
       </c>
-      <c r="R16" s="74" t="s">
+      <c r="R16" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="S16" s="74" t="s">
-        <v>153</v>
-      </c>
-      <c r="T16" s="74" t="s">
-        <v>161</v>
-      </c>
-      <c r="U16" s="74" t="s">
+      <c r="S16" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="T16" s="55" t="s">
         <v>160</v>
+      </c>
+      <c r="U16" s="55" t="s">
+        <v>159</v>
       </c>
       <c r="V16" s="34"/>
     </row>
@@ -2271,10 +2279,10 @@
       </c>
       <c r="E17" s="39"/>
       <c r="F17" s="39"/>
-      <c r="G17" s="38" t="s">
+      <c r="G17" s="58" t="s">
         <v>139</v>
       </c>
-      <c r="H17" s="44">
+      <c r="H17" s="43">
         <v>14</v>
       </c>
       <c r="I17" s="40" t="s">
@@ -2295,22 +2303,22 @@
       <c r="P17" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Q17" s="74">
+      <c r="Q17" s="55">
         <v>7</v>
       </c>
-      <c r="R17" s="74" t="s">
+      <c r="R17" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="S17" s="74" t="s">
+      <c r="S17" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="T17" s="55" t="s">
+        <v>139</v>
+      </c>
+      <c r="U17" s="55" t="s">
         <v>153</v>
       </c>
-      <c r="T17" s="74" t="s">
-        <v>139</v>
-      </c>
-      <c r="U17" s="74" t="s">
-        <v>154</v>
-      </c>
-      <c r="X17" s="48"/>
+      <c r="X17" s="47"/>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" s="40" t="s">
@@ -2327,7 +2335,7 @@
       </c>
       <c r="E18" s="39"/>
       <c r="F18" s="39"/>
-      <c r="G18" s="38" t="s">
+      <c r="G18" s="58" t="s">
         <v>115</v>
       </c>
       <c r="H18" s="40">
@@ -2351,23 +2359,23 @@
       <c r="P18" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Q18" s="74">
+      <c r="Q18" s="55">
         <v>7</v>
       </c>
-      <c r="R18" s="74" t="s">
+      <c r="R18" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="S18" s="74" t="s">
-        <v>153</v>
-      </c>
-      <c r="T18" s="74" t="s">
-        <v>162</v>
-      </c>
-      <c r="U18" s="74" t="s">
-        <v>160</v>
-      </c>
-      <c r="V18" s="75"/>
-      <c r="X18" s="48"/>
+      <c r="S18" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="T18" s="55" t="s">
+        <v>161</v>
+      </c>
+      <c r="U18" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="V18" s="56"/>
+      <c r="X18" s="47"/>
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="s">
@@ -2386,17 +2394,17 @@
         <v>92</v>
       </c>
       <c r="F19" s="39"/>
-      <c r="G19" s="38" t="s">
+      <c r="G19" s="58" t="s">
         <v>140</v>
       </c>
-      <c r="H19" s="44">
+      <c r="H19" s="43">
         <v>16</v>
       </c>
       <c r="I19" s="40" t="s">
         <v>90</v>
       </c>
       <c r="J19" s="39" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="K19" s="40" t="s">
         <v>89</v>
@@ -2410,23 +2418,23 @@
       <c r="P19" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Q19" s="74">
+      <c r="Q19" s="55">
         <v>7</v>
       </c>
-      <c r="R19" s="74" t="s">
+      <c r="R19" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="S19" s="74" t="s">
+      <c r="S19" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="T19" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="U19" s="55" t="s">
         <v>153</v>
       </c>
-      <c r="T19" s="74" t="s">
-        <v>140</v>
-      </c>
-      <c r="U19" s="74" t="s">
-        <v>154</v>
-      </c>
       <c r="V19" s="34"/>
-      <c r="X19" s="48"/>
+      <c r="X19" s="47"/>
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" s="40" t="s">
@@ -2443,10 +2451,10 @@
       </c>
       <c r="E20" s="38"/>
       <c r="F20" s="39"/>
-      <c r="G20" s="38" t="s">
+      <c r="G20" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="H20" s="44">
+      <c r="H20" s="43">
         <v>17</v>
       </c>
       <c r="I20" s="40" t="s">
@@ -2467,23 +2475,23 @@
       <c r="P20" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Q20" s="74">
+      <c r="Q20" s="55">
         <v>7</v>
       </c>
-      <c r="R20" s="74" t="s">
+      <c r="R20" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="S20" s="74" t="s">
+      <c r="S20" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="T20" s="55" t="s">
+        <v>156</v>
+      </c>
+      <c r="U20" s="55" t="s">
         <v>153</v>
       </c>
-      <c r="T20" s="74" t="s">
-        <v>157</v>
-      </c>
-      <c r="U20" s="74" t="s">
-        <v>154</v>
-      </c>
-      <c r="V20" s="45"/>
-      <c r="X20" s="48"/>
+      <c r="V20" s="44"/>
+      <c r="X20" s="47"/>
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" s="40" t="s">
@@ -2502,7 +2510,7 @@
         <v>92</v>
       </c>
       <c r="F21" s="39"/>
-      <c r="G21" s="38" t="s">
+      <c r="G21" s="58" t="s">
         <v>141</v>
       </c>
       <c r="H21" s="40">
@@ -2512,7 +2520,7 @@
         <v>90</v>
       </c>
       <c r="J21" s="39" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K21" s="40" t="s">
         <v>89</v>
@@ -2526,23 +2534,23 @@
       <c r="P21" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Q21" s="74">
+      <c r="Q21" s="55">
         <v>7</v>
       </c>
-      <c r="R21" s="74" t="s">
+      <c r="R21" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="S21" s="74" t="s">
+      <c r="S21" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="T21" s="55" t="s">
+        <v>158</v>
+      </c>
+      <c r="U21" s="55" t="s">
         <v>153</v>
       </c>
-      <c r="T21" s="74" t="s">
-        <v>159</v>
-      </c>
-      <c r="U21" s="74" t="s">
-        <v>154</v>
-      </c>
-      <c r="V21" s="45"/>
-      <c r="X21" s="48"/>
+      <c r="V21" s="44"/>
+      <c r="X21" s="47"/>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22" s="40" t="s">
@@ -2559,10 +2567,10 @@
       </c>
       <c r="E22" s="39"/>
       <c r="F22" s="39"/>
-      <c r="G22" s="38" t="s">
+      <c r="G22" s="58" t="s">
         <v>116</v>
       </c>
-      <c r="H22" s="44">
+      <c r="H22" s="43">
         <v>19</v>
       </c>
       <c r="I22" s="40" t="s">
@@ -2582,28 +2590,28 @@
         <v>79</v>
       </c>
       <c r="O22" s="39" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="P22" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Q22" s="74">
+      <c r="Q22" s="55">
         <v>6</v>
       </c>
-      <c r="R22" s="74" t="s">
+      <c r="R22" s="55" t="s">
+        <v>168</v>
+      </c>
+      <c r="S22" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="S22" s="74" t="s">
-        <v>170</v>
-      </c>
-      <c r="T22" s="52" t="s">
-        <v>174</v>
-      </c>
-      <c r="U22" s="74" t="s">
-        <v>172</v>
+      <c r="T22" s="51" t="s">
+        <v>173</v>
+      </c>
+      <c r="U22" s="55" t="s">
+        <v>171</v>
       </c>
       <c r="V22" s="34"/>
-      <c r="W22" s="47"/>
+      <c r="W22" s="46"/>
     </row>
     <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" s="40" t="s">
@@ -2623,7 +2631,7 @@
       <c r="G23" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="44">
+      <c r="H23" s="43">
         <v>20</v>
       </c>
       <c r="I23" s="40" t="s">
@@ -2642,11 +2650,11 @@
       <c r="P23" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Q23" s="53"/>
-      <c r="R23" s="54"/>
-      <c r="S23" s="54"/>
-      <c r="T23" s="54"/>
-      <c r="U23" s="54"/>
+      <c r="Q23" s="52"/>
+      <c r="R23" s="53"/>
+      <c r="S23" s="53"/>
+      <c r="T23" s="53"/>
+      <c r="U23" s="53"/>
       <c r="V23" s="34"/>
     </row>
     <row r="24" spans="1:38" s="36" customFormat="1" x14ac:dyDescent="0.25">
@@ -2690,22 +2698,22 @@
       <c r="P24" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Q24" s="74">
+      <c r="Q24" s="55">
         <v>6</v>
       </c>
-      <c r="R24" s="74" t="s">
+      <c r="R24" s="55" t="s">
+        <v>168</v>
+      </c>
+      <c r="S24" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="S24" s="74" t="s">
+      <c r="T24" s="51" t="s">
         <v>170</v>
       </c>
-      <c r="T24" s="52" t="s">
+      <c r="U24" s="55" t="s">
         <v>171</v>
       </c>
-      <c r="U24" s="74" t="s">
-        <v>172</v>
-      </c>
-      <c r="V24" s="45"/>
+      <c r="V24" s="44"/>
       <c r="W24" s="34"/>
       <c r="X24" s="34"/>
       <c r="Y24" s="34"/>
@@ -2741,7 +2749,7 @@
       <c r="G25" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="H25" s="44">
+      <c r="H25" s="43">
         <v>22</v>
       </c>
       <c r="I25" s="40" t="s">
@@ -2762,23 +2770,23 @@
       <c r="P25" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Q25" s="74">
+      <c r="Q25" s="55">
         <v>7</v>
       </c>
-      <c r="R25" s="74" t="s">
+      <c r="R25" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="S25" s="74" t="s">
-        <v>153</v>
-      </c>
-      <c r="T25" s="74" t="s">
-        <v>158</v>
-      </c>
-      <c r="U25" s="74" t="s">
-        <v>160</v>
-      </c>
-      <c r="V25" s="75"/>
-      <c r="X25" s="48"/>
+      <c r="S25" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="T25" s="55" t="s">
+        <v>157</v>
+      </c>
+      <c r="U25" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="V25" s="56"/>
+      <c r="X25" s="47"/>
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26" s="40"/>
@@ -2788,7 +2796,7 @@
       <c r="E26" s="39"/>
       <c r="F26" s="39"/>
       <c r="G26" s="38"/>
-      <c r="H26" s="44"/>
+      <c r="H26" s="43"/>
       <c r="I26" s="40"/>
       <c r="J26" s="39"/>
       <c r="K26" s="40"/>
@@ -2802,9 +2810,9 @@
       <c r="S26" s="41"/>
       <c r="T26" s="41"/>
       <c r="U26" s="41"/>
-      <c r="V26" s="45"/>
-      <c r="W26" s="47"/>
-      <c r="X26" s="49"/>
+      <c r="V26" s="44"/>
+      <c r="W26" s="46"/>
+      <c r="X26" s="48"/>
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27" s="40"/>
@@ -2814,7 +2822,7 @@
       <c r="E27" s="39"/>
       <c r="F27" s="39"/>
       <c r="G27" s="38"/>
-      <c r="H27" s="44"/>
+      <c r="H27" s="43"/>
       <c r="I27" s="40"/>
       <c r="J27" s="39"/>
       <c r="K27" s="40"/>
@@ -2828,9 +2836,9 @@
       <c r="S27" s="41"/>
       <c r="T27" s="41"/>
       <c r="U27" s="41"/>
-      <c r="V27" s="45"/>
-      <c r="W27" s="47"/>
-      <c r="X27" s="48"/>
+      <c r="V27" s="44"/>
+      <c r="W27" s="46"/>
+      <c r="X27" s="47"/>
     </row>
     <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28" s="40"/>
@@ -2840,7 +2848,7 @@
       <c r="E28" s="39"/>
       <c r="F28" s="39"/>
       <c r="G28" s="38"/>
-      <c r="H28" s="44"/>
+      <c r="H28" s="43"/>
       <c r="I28" s="40"/>
       <c r="J28" s="39"/>
       <c r="K28" s="40"/>
@@ -2855,7 +2863,7 @@
       <c r="T28" s="41"/>
       <c r="U28" s="41"/>
       <c r="V28" s="34"/>
-      <c r="X28" s="47"/>
+      <c r="X28" s="46"/>
     </row>
     <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29" s="40"/>
@@ -2880,7 +2888,7 @@
       <c r="T29" s="41"/>
       <c r="U29" s="41"/>
       <c r="V29" s="34"/>
-      <c r="W29" s="47"/>
+      <c r="W29" s="46"/>
     </row>
     <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30" s="40"/>
@@ -2890,7 +2898,7 @@
       <c r="E30" s="39"/>
       <c r="F30" s="39"/>
       <c r="G30" s="38"/>
-      <c r="H30" s="44"/>
+      <c r="H30" s="43"/>
       <c r="I30" s="40"/>
       <c r="J30" s="39"/>
       <c r="K30" s="40"/>
@@ -2905,8 +2913,8 @@
       <c r="T30" s="41"/>
       <c r="U30" s="41"/>
       <c r="V30" s="34"/>
-      <c r="W30" s="47"/>
-      <c r="X30" s="50"/>
+      <c r="W30" s="46"/>
+      <c r="X30" s="49"/>
     </row>
     <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31" s="40"/>
@@ -2916,7 +2924,7 @@
       <c r="E31" s="39"/>
       <c r="F31" s="39"/>
       <c r="G31" s="38"/>
-      <c r="H31" s="44"/>
+      <c r="H31" s="43"/>
       <c r="I31" s="40"/>
       <c r="J31" s="39"/>
       <c r="K31" s="40"/>
@@ -2931,7 +2939,7 @@
       <c r="T31" s="41"/>
       <c r="U31" s="41"/>
       <c r="V31" s="34"/>
-      <c r="X31" s="50"/>
+      <c r="X31" s="49"/>
     </row>
     <row r="32" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A32" s="40"/>
@@ -2941,7 +2949,7 @@
       <c r="E32" s="39"/>
       <c r="F32" s="39"/>
       <c r="G32" s="38"/>
-      <c r="H32" s="44"/>
+      <c r="H32" s="43"/>
       <c r="I32" s="40"/>
       <c r="J32" s="39"/>
       <c r="K32" s="40"/>
@@ -2956,7 +2964,7 @@
       <c r="T32" s="41"/>
       <c r="U32" s="41"/>
       <c r="V32" s="34"/>
-      <c r="X32" s="48"/>
+      <c r="X32" s="47"/>
       <c r="Y32" s="42"/>
     </row>
     <row r="33" spans="1:39" x14ac:dyDescent="0.25">
@@ -2967,7 +2975,7 @@
       <c r="E33" s="39"/>
       <c r="F33" s="39"/>
       <c r="G33" s="38"/>
-      <c r="H33" s="44"/>
+      <c r="H33" s="43"/>
       <c r="I33" s="40"/>
       <c r="J33" s="39"/>
       <c r="K33" s="40"/>
@@ -2982,7 +2990,7 @@
       <c r="T33" s="41"/>
       <c r="U33" s="41"/>
       <c r="V33" s="34"/>
-      <c r="X33" s="48"/>
+      <c r="X33" s="47"/>
     </row>
     <row r="34" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A34" s="40"/>
@@ -2992,7 +3000,7 @@
       <c r="E34" s="39"/>
       <c r="F34" s="39"/>
       <c r="G34" s="38"/>
-      <c r="H34" s="44"/>
+      <c r="H34" s="43"/>
       <c r="I34" s="40"/>
       <c r="J34" s="39"/>
       <c r="K34" s="40"/>
@@ -3007,8 +3015,8 @@
       <c r="T34" s="41"/>
       <c r="U34" s="41"/>
       <c r="V34" s="34"/>
-      <c r="W34" s="47"/>
-      <c r="X34" s="48"/>
+      <c r="W34" s="46"/>
+      <c r="X34" s="47"/>
     </row>
     <row r="35" spans="1:39" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="40"/>
@@ -3018,7 +3026,7 @@
       <c r="E35" s="39"/>
       <c r="F35" s="39"/>
       <c r="G35" s="38"/>
-      <c r="H35" s="44"/>
+      <c r="H35" s="43"/>
       <c r="I35" s="40"/>
       <c r="J35" s="39"/>
       <c r="K35" s="40"/>
@@ -3032,8 +3040,8 @@
       <c r="S35" s="41"/>
       <c r="T35" s="41"/>
       <c r="U35" s="41"/>
-      <c r="W35" s="47"/>
-      <c r="X35" s="50"/>
+      <c r="W35" s="46"/>
+      <c r="X35" s="49"/>
     </row>
     <row r="36" spans="1:39" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="40"/>
@@ -3043,7 +3051,7 @@
       <c r="E36" s="39"/>
       <c r="F36" s="39"/>
       <c r="G36" s="38"/>
-      <c r="H36" s="44"/>
+      <c r="H36" s="43"/>
       <c r="I36" s="40"/>
       <c r="J36" s="39"/>
       <c r="K36" s="40"/>
@@ -3057,7 +3065,7 @@
       <c r="S36" s="41"/>
       <c r="T36" s="41"/>
       <c r="U36" s="41"/>
-      <c r="V36" s="45"/>
+      <c r="V36" s="44"/>
       <c r="W36" s="34"/>
       <c r="X36" s="34"/>
       <c r="Y36" s="34"/>
@@ -3084,7 +3092,7 @@
       <c r="E37" s="39"/>
       <c r="F37" s="39"/>
       <c r="G37" s="38"/>
-      <c r="H37" s="44"/>
+      <c r="H37" s="43"/>
       <c r="I37" s="40"/>
       <c r="J37" s="39"/>
       <c r="K37" s="40"/>
@@ -3099,8 +3107,8 @@
       <c r="T37" s="41"/>
       <c r="U37" s="41"/>
       <c r="V37" s="34"/>
-      <c r="W37" s="47"/>
-      <c r="X37" s="50"/>
+      <c r="W37" s="46"/>
+      <c r="X37" s="49"/>
       <c r="Y37" s="34"/>
       <c r="Z37" s="34"/>
       <c r="AA37" s="34"/>
@@ -3125,7 +3133,7 @@
       <c r="E38" s="39"/>
       <c r="F38" s="39"/>
       <c r="G38" s="38"/>
-      <c r="H38" s="44"/>
+      <c r="H38" s="43"/>
       <c r="I38" s="40"/>
       <c r="J38" s="39"/>
       <c r="K38" s="40"/>
@@ -3140,7 +3148,7 @@
       <c r="T38" s="41"/>
       <c r="U38" s="41"/>
       <c r="V38" s="34"/>
-      <c r="X38" s="48"/>
+      <c r="X38" s="47"/>
     </row>
     <row r="39" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A39" s="40"/>
@@ -3150,7 +3158,7 @@
       <c r="E39" s="39"/>
       <c r="F39" s="39"/>
       <c r="G39" s="38"/>
-      <c r="H39" s="44"/>
+      <c r="H39" s="43"/>
       <c r="I39" s="40"/>
       <c r="J39" s="39"/>
       <c r="K39" s="40"/>
@@ -3189,8 +3197,8 @@
       <c r="T40" s="41"/>
       <c r="U40" s="41"/>
       <c r="V40" s="34"/>
-      <c r="W40" s="47"/>
-      <c r="X40" s="48"/>
+      <c r="W40" s="46"/>
+      <c r="X40" s="47"/>
       <c r="Y40" s="42"/>
     </row>
     <row r="41" spans="1:39" s="34" customFormat="1" x14ac:dyDescent="0.25">
@@ -6411,7 +6419,7 @@
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="Q1:Q2"/>
   </mergeCells>
-  <dataValidations count="5">
+  <dataValidations disablePrompts="1" count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K40">
       <formula1>$C$43:$D$43</formula1>
     </dataValidation>

</xml_diff>